<commit_message>
Forgot to update timesheet
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -100,6 +100,7 @@
   <fonts count="4">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -185,15 +186,15 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A47" activeCellId="0" pane="topLeft" sqref="A47"/>
+      <selection activeCell="C4" activeCellId="0" pane="topLeft" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.3843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1803921568627"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.3607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -231,6 +232,9 @@
       <c r="B3" s="2" t="n">
         <v>41213</v>
       </c>
+      <c r="C3" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
@@ -259,7 +263,7 @@
         <v>41216</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
@@ -277,7 +281,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="n">
         <f aca="false">SUM(C2:C7)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -608,7 +612,7 @@
       </c>
       <c r="C46" s="1" t="n">
         <f aca="false">SUM(C44,C40,C32,C24,C16,C8)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -629,17 +633,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -654,17 +658,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Started removing semantic actions from y files, and compiling into plgs
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -186,18 +186,18 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
+      <selection activeCell="C20" activeCellId="0" pane="topLeft" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.5529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8470588235294"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.9333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -214,7 +214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -225,7 +225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
@@ -239,7 +239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -247,7 +247,7 @@
         <v>41214</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>9</v>
       </c>
@@ -255,7 +255,7 @@
         <v>41215</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
@@ -263,7 +263,7 @@
         <v>41216</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
@@ -274,7 +274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
@@ -284,7 +284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
@@ -292,7 +292,7 @@
         <v>41218</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>5</v>
       </c>
@@ -303,7 +303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>6</v>
       </c>
@@ -311,7 +311,7 @@
         <v>41220</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>8</v>
       </c>
@@ -319,7 +319,7 @@
         <v>41221</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>9</v>
       </c>
@@ -327,7 +327,7 @@
         <v>41222</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>10</v>
       </c>
@@ -335,7 +335,7 @@
         <v>41223</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>11</v>
       </c>
@@ -346,7 +346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>13</v>
       </c>
@@ -356,7 +356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>14</v>
       </c>
@@ -364,23 +364,29 @@
         <v>41225</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>41226</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="C18" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>41227</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="C19" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>8</v>
       </c>
@@ -388,7 +394,7 @@
         <v>41228</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>9</v>
       </c>
@@ -396,7 +402,7 @@
         <v>41229</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>10</v>
       </c>
@@ -404,7 +410,7 @@
         <v>41230</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>11</v>
       </c>
@@ -418,17 +424,17 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>14</v>
       </c>
@@ -436,7 +442,7 @@
         <v>41232</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>5</v>
       </c>
@@ -444,7 +450,7 @@
         <v>41233</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>6</v>
       </c>
@@ -452,7 +458,7 @@
         <v>41234</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>8</v>
       </c>
@@ -460,7 +466,7 @@
         <v>41235</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>9</v>
       </c>
@@ -468,7 +474,7 @@
         <v>41236</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>10</v>
       </c>
@@ -476,7 +482,7 @@
         <v>41237</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>11</v>
       </c>
@@ -490,7 +496,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>13</v>
       </c>
@@ -500,7 +506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>14</v>
       </c>
@@ -508,7 +514,7 @@
         <v>41239</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>5</v>
       </c>
@@ -516,7 +522,7 @@
         <v>41240</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>6</v>
       </c>
@@ -524,7 +530,7 @@
         <v>41241</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>8</v>
       </c>
@@ -532,7 +538,7 @@
         <v>41242</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>9</v>
       </c>
@@ -540,7 +546,7 @@
         <v>41243</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>10</v>
       </c>
@@ -548,7 +554,7 @@
         <v>41244</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>11</v>
       </c>
@@ -559,7 +565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
         <v>13</v>
       </c>
@@ -569,7 +575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
         <v>14</v>
       </c>
@@ -580,7 +586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
         <v>5</v>
       </c>
@@ -588,7 +594,7 @@
         <v>41247</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
         <v>6</v>
       </c>
@@ -599,7 +605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
         <v>13</v>
       </c>
@@ -609,13 +615,13 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
         <v>22</v>
       </c>
       <c r="C46" s="1" t="n">
         <f aca="false">SUM(C44,C40,C32,C24,C16,C8)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +647,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -666,7 +672,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>